<commit_message>
Add new request for event permit in JSON and update Excel file
</commit_message>
<xml_diff>
--- a/data/ÜbersichtGesucheUndInformationen.xlsx
+++ b/data/ÜbersichtGesucheUndInformationen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csp\Workspace\Other\Hackaton25\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADE0BAE-141D-4B7B-BEAA-CC92B24DEF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66343ED-FA13-41AD-9FD0-575E89DC932A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{42EC53E2-04FD-422E-B64F-FCCDEFC4C07C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
   <si>
     <t>Kategorie</t>
   </si>
@@ -561,13 +561,28 @@
   </si>
   <si>
     <t>Zustaendigkeit</t>
+  </si>
+  <si>
+    <t>Gesuch Grossanlass Andermatt</t>
+  </si>
+  <si>
+    <t>https://www.gemeinde-andermatt.ch/verwaltung/online-schalter.html/70</t>
+  </si>
+  <si>
+    <t>https://www.gemeinde-andermatt.ch/public/upload/assets/690/Grossanlassgesuch_Gemeinde.pdf?fp=1542959697356</t>
+  </si>
+  <si>
+    <t>Andermatt</t>
+  </si>
+  <si>
+    <t>041 880 71 41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -579,6 +594,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Roboto"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -604,10 +626,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -624,8 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,11 +985,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B914F4E-8582-44DA-852F-25295B786F55}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -1860,9 +1887,43 @@
         <v>164</v>
       </c>
     </row>
+    <row r="35" spans="1:9" ht="78.75" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I34" xr:uid="{8B914F4E-8582-44DA-852F-25295B786F55}"/>
+  <hyperlinks>
+    <hyperlink ref="E35" r:id="rId1" xr:uid="{1850BB0C-9E9A-403C-8D0F-CAAEB886FF55}"/>
+    <hyperlink ref="D35" r:id="rId2" xr:uid="{AD6CFDC5-CBC0-4B66-A23C-6DC1108BB7C5}"/>
+    <hyperlink ref="H35" r:id="rId3" xr:uid="{15F7CFDD-D37A-4E9F-B2A9-E90596F6902E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>